<commit_message>
finish homework week 2
</commit_message>
<xml_diff>
--- a/01需求调研/调研资料目录.xlsx
+++ b/01需求调研/调研资料目录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bjut\2020_VR\vr_Git\vr_indoorFurnitureRoaming\01需求调研\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABA69AD-4AB2-45B7-9C9E-59C90A77F41E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6253CEE7-22B7-46E7-8ED9-26E578C7BF67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="3825" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="3885" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>[参考]卧室图</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>https://github.com/MuzhiYing/vr_indoorFurnitureRoaming/blob/master/01%E9%9C%80%E6%B1%82%E8%B0%83%E7%A0%94/%E5%AE%A4%E5%86%85%E6%BC%AB%E6%B8%B8_%E9%9C%80%E6%B1%82%E8%A7%84%E6%A0%BC%E8%AF%B4%E6%98%8E%E4%B9%A6.docx</t>
+  </si>
+  <si>
+    <t>[参考]厨房.zip</t>
+  </si>
+  <si>
+    <t>[参考]客厅.rar</t>
+  </si>
+  <si>
+    <t>https://github.com/MuzhiYing/vr_indoorFurnitureRoaming/blob/master/01%E9%9C%80%E6%B1%82%E8%B0%83%E7%A0%94/%E9%99%84%E5%BD%95/%5B%E5%8F%82%E8%80%83%5D%E5%AE%A2%E5%8E%85.rar</t>
+  </si>
+  <si>
+    <t>https://github.com/MuzhiYing/vr_indoorFurnitureRoaming/blob/master/01%E9%9C%80%E6%B1%82%E8%B0%83%E7%A0%94/%E9%99%84%E5%BD%95/%5B%E5%8F%82%E8%80%83%5D%E5%8E%A8%E6%88%BF.zip</t>
   </si>
 </sst>
 </file>
@@ -532,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -621,12 +633,20 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
@@ -736,8 +756,10 @@
     <hyperlink ref="B18" r:id="rId9" xr:uid="{0AC6789E-E97A-4F95-A71C-8C6D20B81D85}"/>
     <hyperlink ref="B19" r:id="rId10" xr:uid="{E10D912C-E13B-4661-B499-571EAFC4C6E6}"/>
     <hyperlink ref="B20" r:id="rId11" xr:uid="{D162E66A-CC5A-4090-B0C5-9D80862F8D43}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{9C1E12B3-E77F-4AC1-B638-90C2F56F5AD8}"/>
+    <hyperlink ref="B11" r:id="rId13" xr:uid="{46E84AF0-CA32-4299-B588-EB3F31BDFF11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>